<commit_message>
debugging and final design
</commit_message>
<xml_diff>
--- a/medical_descriptions_conclusions - Copy.xlsx
+++ b/medical_descriptions_conclusions - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379307B5-4680-4A4B-B63C-06ABF642FBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678C8644-3452-4599-856C-6B81CDC51087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="130">
   <si>
     <t>Acne</t>
   </si>
@@ -458,10 +458,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B938"/>
+  <dimension ref="A1:B939"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -724,35 +725,35 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
+      <c r="B5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>45</v>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>47</v>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -760,7 +761,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -768,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -776,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -784,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -792,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -800,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -808,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -816,7 +817,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -824,39 +825,39 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
-        <v>58</v>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
-        <v>59</v>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -864,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -872,7 +873,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -880,7 +881,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -888,7 +889,7 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -896,7 +897,7 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -904,55 +905,55 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B29" t="s">
-        <v>66</v>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B31" t="s">
-        <v>67</v>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B33" t="s">
-        <v>68</v>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -960,7 +961,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -968,7 +969,7 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -976,39 +977,39 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B38" t="s">
-        <v>72</v>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>73</v>
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B40" t="s">
-        <v>74</v>
+      <c r="B40" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1016,7 +1017,7 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1024,7 +1025,7 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1040,7 +1041,7 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1048,55 +1049,55 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>79</v>
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B47" t="s">
-        <v>80</v>
+      <c r="B47" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B49" t="s">
-        <v>81</v>
+      <c r="B49" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B51" t="s">
-        <v>82</v>
+      <c r="B51" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1104,7 +1105,7 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1112,31 +1113,31 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B54" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B56" t="s">
-        <v>86</v>
+      <c r="B56" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1144,23 +1145,23 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>85</v>
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B59" t="s">
-        <v>88</v>
+      <c r="B59" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1168,55 +1169,55 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B64" t="s">
-        <v>91</v>
+      <c r="B64" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>92</v>
+        <v>17</v>
+      </c>
+      <c r="B65" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B66" t="s">
-        <v>93</v>
+      <c r="B66" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1224,143 +1225,143 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>95</v>
+        <v>18</v>
+      </c>
+      <c r="B68" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B69" t="s">
-        <v>96</v>
+      <c r="B69" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="B70" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B72" t="s">
-        <v>98</v>
+      <c r="B72" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>99</v>
+        <v>22</v>
+      </c>
+      <c r="B73" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B74" t="s">
-        <v>100</v>
+      <c r="B74" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B75" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B80" t="s">
-        <v>101</v>
+      <c r="B80" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B81" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B82" t="s">
-        <v>102</v>
+      <c r="B82" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B83" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B84" t="s">
-        <v>103</v>
+      <c r="B84" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1368,7 +1369,7 @@
         <v>28</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1376,7 +1377,7 @@
         <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1384,7 +1385,7 @@
         <v>28</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1392,7 +1393,7 @@
         <v>28</v>
       </c>
       <c r="B88" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1400,7 +1401,7 @@
         <v>28</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1408,95 +1409,95 @@
         <v>28</v>
       </c>
       <c r="B90" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="B91" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B92" t="s">
-        <v>110</v>
+      <c r="B92" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B93" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B94" t="s">
-        <v>111</v>
+      <c r="B94" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="B95" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B97" t="s">
-        <v>103</v>
+      <c r="B97" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B98" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B99" t="s">
-        <v>112</v>
+      <c r="B99" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>113</v>
+      <c r="B100" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B101" t="s">
-        <v>114</v>
+      <c r="B101" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1504,7 +1505,7 @@
         <v>34</v>
       </c>
       <c r="B102" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1512,7 +1513,7 @@
         <v>34</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1520,7 +1521,7 @@
         <v>34</v>
       </c>
       <c r="B104" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1528,7 +1529,7 @@
         <v>34</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1536,7 +1537,7 @@
         <v>34</v>
       </c>
       <c r="B106" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1544,7 +1545,7 @@
         <v>34</v>
       </c>
       <c r="B107" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1552,7 +1553,7 @@
         <v>34</v>
       </c>
       <c r="B108" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1560,15 +1561,15 @@
         <v>34</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B110" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1576,23 +1577,23 @@
         <v>35</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>119</v>
+        <v>35</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B112" t="s">
-        <v>120</v>
+      <c r="B112" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B113" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1600,23 +1601,23 @@
         <v>36</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B115" t="s">
-        <v>122</v>
+      <c r="B115" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B116" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1631,16 +1632,16 @@
       <c r="A118" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B118" t="s">
-        <v>123</v>
+      <c r="B118" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B119" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1648,15 +1649,15 @@
         <v>38</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B121" t="s">
-        <v>125</v>
+      <c r="B121" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1664,7 +1665,7 @@
         <v>38</v>
       </c>
       <c r="B122" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1672,10 +1673,17 @@
         <v>38</v>
       </c>
       <c r="B123" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B124" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="125" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="126" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="127" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2490,6 +2498,7 @@
     <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>